<commit_message>
Post WGP - Pre-mini expac update
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/CalamityMeta.xlsx
+++ b/Excel_and_CSV/CalamityMeta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9063BF76-E632-45B2-8FDF-D0A2C2629F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A739A5-6290-4CDA-8E66-885E183F889D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="235">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -68,9 +68,6 @@
     <t>76QHo</t>
   </si>
   <si>
-    <t>Combo Forest</t>
-  </si>
-  <si>
     <t>Ladica, Verdant Claw</t>
   </si>
   <si>
@@ -359,12 +356,6 @@
     <t>745MY</t>
   </si>
   <si>
-    <t>Ceres, Bride of the Night</t>
-  </si>
-  <si>
-    <t>7BqzI</t>
-  </si>
-  <si>
     <t>Last Words Shadow</t>
   </si>
   <si>
@@ -608,18 +599,6 @@
     <t>7I-Ew</t>
   </si>
   <si>
-    <t>Abysmal Wraith</t>
-  </si>
-  <si>
-    <t>747oy</t>
-  </si>
-  <si>
-    <t>Linkstaff Necromancer</t>
-  </si>
-  <si>
-    <t>7FXnY</t>
-  </si>
-  <si>
     <t>Control Forest</t>
   </si>
   <si>
@@ -650,15 +629,6 @@
     <t>7G1X6</t>
   </si>
   <si>
-    <t>Ceres OTK Shadow</t>
-  </si>
-  <si>
-    <t>Great Mother's Embrace</t>
-  </si>
-  <si>
-    <t>7Dlmg</t>
-  </si>
-  <si>
     <t>Crystal Witch</t>
   </si>
   <si>
@@ -705,6 +675,57 @@
   </si>
   <si>
     <t>Frigg</t>
+  </si>
+  <si>
+    <t>Djeana, the Stouthearted</t>
+  </si>
+  <si>
+    <t>7FEFY</t>
+  </si>
+  <si>
+    <t>Blazing Dragonewt</t>
+  </si>
+  <si>
+    <t>7IzW2</t>
+  </si>
+  <si>
+    <t>Erika, Loyal Swordsavant</t>
+  </si>
+  <si>
+    <t>7EVt6</t>
+  </si>
+  <si>
+    <t>Aggro Ladica Forest</t>
+  </si>
+  <si>
+    <t>Combo Ladica Forest</t>
+  </si>
+  <si>
+    <t>Phantombloom Predator</t>
+  </si>
+  <si>
+    <t>7Hsj6</t>
+  </si>
+  <si>
+    <t>Sen, Stormclaw Cat</t>
+  </si>
+  <si>
+    <t>76SkM</t>
+  </si>
+  <si>
+    <t>Suzy Shadow</t>
+  </si>
+  <si>
+    <t>Suzy, Hexcaster</t>
+  </si>
+  <si>
+    <t>7JQpC</t>
+  </si>
+  <si>
+    <t>Cernunnos</t>
+  </si>
+  <si>
+    <t>7JTFc</t>
   </si>
 </sst>
 </file>
@@ -722,32 +743,38 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -998,10 +1025,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I997"/>
+  <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1027,19 +1054,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I1" s="2"/>
     </row>
@@ -1097,48 +1124,48 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>225</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>9</v>
+        <v>226</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>9</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>9</v>
@@ -1149,16 +1176,16 @@
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>13</v>
@@ -1175,360 +1202,360 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>9</v>
+        <v>228</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>9</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="G8" s="5" t="s">
-        <v>9</v>
+        <v>228</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="H12" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    </row>
+    <row r="14" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="E15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="G15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>50</v>
+        <v>222</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>53</v>
+        <v>223</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>222</v>
+        <v>44</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>223</v>
+        <v>45</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>213</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="3" t="s">
+    </row>
+    <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="B19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>64</v>
+        <v>43</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>9</v>
+        <v>202</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>9</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>9</v>
@@ -1537,24 +1564,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>72</v>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>66</v>
+        <v>43</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>9</v>
@@ -1562,26 +1589,25 @@
       <c r="H21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>9</v>
@@ -1589,159 +1615,160 @@
       <c r="H22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E26" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="B28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H28" s="3" t="s">
@@ -1750,24 +1777,24 @@
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>100</v>
+        <v>77</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="G29" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H29" s="3" t="s">
@@ -1776,22 +1803,22 @@
     </row>
     <row r="30" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>216</v>
+        <v>86</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>9</v>
@@ -1802,75 +1829,75 @@
     </row>
     <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F31" s="3" t="s">
+      <c r="D32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="B33" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="D33" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="G33" s="3" t="s">
         <v>9</v>
       </c>
@@ -1878,24 +1905,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>119</v>
+    <row r="34" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>230</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>121</v>
+        <v>231</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>122</v>
+        <v>232</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>121</v>
+        <v>233</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>122</v>
+        <v>234</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>9</v>
@@ -1906,22 +1933,22 @@
     </row>
     <row r="35" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>123</v>
+        <v>206</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>9</v>
@@ -1932,22 +1959,22 @@
     </row>
     <row r="36" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>130</v>
+        <v>107</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>9</v>
@@ -1958,22 +1985,22 @@
     </row>
     <row r="37" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>191</v>
+        <v>118</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>192</v>
+        <v>119</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>207</v>
+        <v>118</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>208</v>
+        <v>119</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>9</v>
@@ -1984,48 +2011,48 @@
     </row>
     <row r="38" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>58</v>
+        <v>122</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>139</v>
+        <v>126</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>9</v>
@@ -2036,22 +2063,22 @@
     </row>
     <row r="40" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>93</v>
+        <v>188</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>94</v>
+        <v>189</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>142</v>
+        <v>200</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>143</v>
+        <v>201</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>9</v>
@@ -2062,74 +2089,74 @@
     </row>
     <row r="41" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>227</v>
+        <v>56</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>226</v>
+        <v>57</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>224</v>
+        <v>130</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>225</v>
+        <v>131</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>9</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>149</v>
+        <v>134</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>142</v>
+        <v>9</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>151</v>
+        <v>92</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>152</v>
+        <v>93</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>9</v>
@@ -2140,22 +2167,22 @@
     </row>
     <row r="44" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>160</v>
+        <v>217</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>160</v>
+        <v>214</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>161</v>
+        <v>215</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>9</v>
@@ -2166,74 +2193,74 @@
     </row>
     <row r="45" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>9</v>
+        <v>139</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>9</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="B47" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F46" s="3" t="s">
+      <c r="E47" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>9</v>
@@ -2244,22 +2271,22 @@
     </row>
     <row r="48" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>9</v>
@@ -2270,22 +2297,22 @@
     </row>
     <row r="49" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>9</v>
@@ -2294,24 +2321,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>169</v>
+        <v>205</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>171</v>
+        <v>138</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>172</v>
+        <v>56</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>9</v>
@@ -2322,22 +2349,22 @@
     </row>
     <row r="51" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="F51" s="3" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>9</v>
@@ -2348,22 +2375,22 @@
     </row>
     <row r="52" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>166</v>
-      </c>
       <c r="F52" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>9</v>
@@ -2374,22 +2401,22 @@
     </row>
     <row r="53" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>9</v>
@@ -2400,38 +2427,107 @@
     </row>
     <row r="54" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C54" t="s">
-        <v>217</v>
-      </c>
-      <c r="D54" t="s">
-        <v>218</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B55" s="7"/>
+      <c r="F55" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="56" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B56" s="7"/>
+      <c r="A56" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="57" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B57" s="7"/>
+      <c r="A57" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C57" t="s">
+        <v>207</v>
+      </c>
+      <c r="D57" t="s">
+        <v>208</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="58" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B58" s="7"/>
@@ -5252,6 +5348,15 @@
     </row>
     <row r="997" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B997" s="7"/>
+    </row>
+    <row r="998" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B998" s="7"/>
+    </row>
+    <row r="999" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B999" s="7"/>
+    </row>
+    <row r="1000" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1000" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5262,7 +5367,7 @@
           <x14:formula1>
             <xm:f>Class!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B997</xm:sqref>
+          <xm:sqref>B2:B1000</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5283,7 +5388,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -5293,37 +5398,37 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for Omen of Storms
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/CalamityMeta.xlsx
+++ b/Excel_and_CSV/CalamityMeta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A739A5-6290-4CDA-8E66-885E183F889D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAC582F-98EE-4A2D-BAC1-60F06A65B516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,12 +452,6 @@
     <t>Ward Haven</t>
   </si>
   <si>
-    <t>Anvelt, Judgment's Cannon</t>
-  </si>
-  <si>
-    <t>74zWS</t>
-  </si>
-  <si>
     <t>Holy Saber</t>
   </si>
   <si>
@@ -539,12 +533,6 @@
     <t>Puppet Portal</t>
   </si>
   <si>
-    <t>Licht, the Gear Magus</t>
-  </si>
-  <si>
-    <t>7Ka2Y</t>
-  </si>
-  <si>
     <t>Stringmaster</t>
   </si>
   <si>
@@ -707,12 +695,6 @@
     <t>7Hsj6</t>
   </si>
   <si>
-    <t>Sen, Stormclaw Cat</t>
-  </si>
-  <si>
-    <t>76SkM</t>
-  </si>
-  <si>
     <t>Suzy Shadow</t>
   </si>
   <si>
@@ -726,6 +708,24 @@
   </si>
   <si>
     <t>7JTFc</t>
+  </si>
+  <si>
+    <t>Imagination Realized</t>
+  </si>
+  <si>
+    <t>7Igiw</t>
+  </si>
+  <si>
+    <t>Young Threadmaster</t>
+  </si>
+  <si>
+    <t>7KVAC</t>
+  </si>
+  <si>
+    <t>74sBi</t>
+  </si>
+  <si>
+    <t>Enchanted Knight</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1028,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1054,19 +1054,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="I1" s="2"/>
     </row>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
@@ -1142,30 +1142,30 @@
         <v>18</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>9</v>
@@ -1176,16 +1176,16 @@
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>13</v>
@@ -1219,11 +1219,11 @@
       <c r="F7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>229</v>
+      <c r="G7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1245,16 +1245,16 @@
       <c r="F8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>229</v>
+      <c r="G8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
@@ -1384,22 +1384,22 @@
     </row>
     <row r="14" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>9</v>
@@ -1410,7 +1410,7 @@
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>27</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="16" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>27</v>
@@ -1448,10 +1448,10 @@
         <v>31</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>9</v>
@@ -1460,7 +1460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
@@ -1474,15 +1474,15 @@
         <v>45</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>44</v>
+        <v>229</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1526,16 +1526,16 @@
         <v>55</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1711,10 +1711,10 @@
         <v>79</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>9</v>
@@ -1737,10 +1737,10 @@
         <v>79</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>9</v>
@@ -1821,10 +1821,10 @@
         <v>90</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1841,10 +1841,10 @@
         <v>93</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>9</v>
@@ -1899,30 +1899,30 @@
         <v>115</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>9</v>
+        <v>225</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>9</v>
+        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>9</v>
@@ -1933,7 +1933,7 @@
     </row>
     <row r="35" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>97</v>
@@ -2069,16 +2069,16 @@
         <v>117</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>9</v>
@@ -2173,16 +2173,16 @@
         <v>138</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>9</v>
@@ -2199,16 +2199,16 @@
         <v>138</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="F45" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>139</v>
@@ -2219,22 +2219,22 @@
     </row>
     <row r="46" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>138</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>9</v>
@@ -2245,22 +2245,22 @@
     </row>
     <row r="47" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>138</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>9</v>
@@ -2269,24 +2269,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>152</v>
+        <v>201</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>154</v>
+      <c r="C48" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>153</v>
+        <v>56</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>154</v>
+        <v>57</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>9</v>
@@ -2297,22 +2297,22 @@
     </row>
     <row r="49" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>138</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>9</v>
@@ -2321,24 +2321,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>205</v>
+        <v>150</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>146</v>
+      <c r="C50" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>57</v>
+        <v>153</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>9</v>
@@ -2349,22 +2349,22 @@
     </row>
     <row r="51" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>9</v>
@@ -2375,22 +2375,22 @@
     </row>
     <row r="52" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C52" s="3" t="s">
+      <c r="D52" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="F52" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>9</v>
@@ -2401,22 +2401,22 @@
     </row>
     <row r="53" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C53" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="F53" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>9</v>
@@ -2427,22 +2427,22 @@
     </row>
     <row r="54" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>9</v>
@@ -2453,22 +2453,22 @@
     </row>
     <row r="55" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>9</v>
@@ -2479,22 +2479,22 @@
     </row>
     <row r="56" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F56" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>9</v>
@@ -2505,22 +2505,22 @@
     </row>
     <row r="57" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C57" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D57" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>9</v>
@@ -5388,7 +5388,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -5428,7 +5428,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>